<commit_message>
update readme and template
</commit_message>
<xml_diff>
--- a/data/smiles/library2.xlsx
+++ b/data/smiles/library2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gary/Downloads/zivi/git/delt-core/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gary/Downloads/zivi/git/delt-core/data/smiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4531347C-EBB9-5F45-8E4F-9DCBC4CC406D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0C4F16-39FA-0247-9E29-E0B0A3B87390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14400" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="581">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="580">
   <si>
     <t>ID</t>
   </si>
@@ -1760,9 +1760,6 @@
   </si>
   <si>
     <t>Complement</t>
-  </si>
-  <si>
-    <t>Special</t>
   </si>
   <si>
     <t>GTGATCCTAC{codon}GCGACCGTGCAGAGC</t>
@@ -1772,7 +1769,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1821,12 +1818,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="6.5"/>
-      <color rgb="FF000000"/>
-      <name val="Courier New"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1859,7 +1850,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1874,12 +1865,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2101,7 +2086,7 @@
       <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -2112,7 +2097,7 @@
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>85</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -5285,53 +5270,37 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.83203125" customWidth="1"/>
-    <col min="16384" max="16384" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="36.83203125" customWidth="1"/>
+    <col min="16382" max="16384" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>576</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="D1" s="2" t="s">
         <v>578</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+      <c r="B2">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>580</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>